<commit_message>
insert with excel check for null or empty cells
</commit_message>
<xml_diff>
--- a/CallManagement_Insert.xlsx
+++ b/CallManagement_Insert.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\production_user19\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\production_user19\source\repos\Insert or Updating CallManagement DB from Excel sheet\Updating DB from uploaded excel_solution\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C641E8C2-E9D3-47B7-862F-795CCAC3CB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F595226E-1244-47E8-AC2E-CBA09E6521DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="1350" windowWidth="25515" windowHeight="12345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Φύλλο1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>CallsId</t>
   </si>
@@ -48,7 +48,10 @@
     <t>ModifiedDate</t>
   </si>
   <si>
-    <t>foo</t>
+    <t>catching null values</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -367,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,19 +402,39 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <v>44594</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
       </c>
       <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>44652</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>